<commit_message>
se5 lite tune power on sequence
Change-Id: I5ce7a61c6dabda35e542fba844704ae0914d86a2

Former-commit-id: e6a687452331efbf9dd0dd1d8f7b1cd15816ddb7
</commit_message>
<xml_diff>
--- a/SE5LITE/config.xlsx
+++ b/SE5LITE/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="17415" tabRatio="500" activeTab="1"/>
+    <workbookView windowHeight="17850" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="148">
   <si>
     <t>Pin number</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>USB-5V</t>
+  </si>
+  <si>
+    <t>U5V</t>
   </si>
   <si>
     <t>ASM3142-3.3V</t>
@@ -470,8 +473,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -503,11 +506,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -519,21 +534,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -541,22 +573,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -570,59 +589,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,8 +611,44 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -678,7 +681,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,19 +801,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,7 +831,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,67 +843,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,67 +855,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -896,15 +899,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -916,36 +910,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -984,140 +948,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="9" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
@@ -1548,8 +1551,8 @@
   <sheetPr/>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1716,13 +1719,13 @@
         <v>14</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="16"/>
     </row>
@@ -2736,11 +2739,11 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G49">
       <formula1>"PP,OD"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D49">
+      <formula1>"INPUT,OUTPUT,AF,ANALOG,NA"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F49">
       <formula1>"NO-PULL,PULL-UP,PULL-DOWN"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D49">
-      <formula1>"INPUT,OUTPUT,AF,ANALOG,NA"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="A1 E1:I1 B2:B37 E2:E49 I2:I49"/>
   </dataValidations>
@@ -2755,8 +2758,8 @@
   <sheetPr/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -3108,10 +3111,10 @@
         <v>138</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
@@ -3119,7 +3122,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>41</v>
@@ -3133,7 +3136,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>71</v>
@@ -3182,22 +3185,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
start wol after power on
Change-Id: I9f67611beed0b6b20f400983ade0e3aadf24e5bf

Former-commit-id: 4314dd5fd0c04e86232c36f6b468ed6d92cea60b
</commit_message>
<xml_diff>
--- a/SE5LITE/config.xlsx
+++ b/SE5LITE/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="17850" tabRatio="500"/>
+    <workbookView windowHeight="17415" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" r:id="rId1"/>
@@ -506,23 +506,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -533,31 +533,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -573,61 +558,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -647,12 +601,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -681,7 +681,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,19 +777,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,13 +807,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +819,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,121 +855,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,11 +890,70 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -914,17 +973,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -939,188 +987,140 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="9" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
@@ -1551,8 +1551,8 @@
   <sheetPr/>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1747,7 +1747,7 @@
         <v>14</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>16</v>
@@ -2739,11 +2739,11 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G49">
       <formula1>"PP,OD"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F49">
+      <formula1>"NO-PULL,PULL-UP,PULL-DOWN"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D49">
       <formula1>"INPUT,OUTPUT,AF,ANALOG,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F49">
-      <formula1>"NO-PULL,PULL-UP,PULL-DOWN"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="A1 E1:I1 B2:B37 E2:E49 I2:I49"/>
   </dataValidations>

</xml_diff>